<commit_message>
added print stuff to it
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hahndol/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hahndol/Documents/School/ComputerScience/Sudoku/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E45963B-BE4D-E540-800D-583C486BD173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1B0A10-0356-F14D-8A30-18496512D929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30460" windowHeight="15880" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30460" windowHeight="15880" activeTab="1" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="40">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -343,6 +343,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -363,9 +366,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -684,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="150" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C41"/>
     </sheetView>
   </sheetViews>
@@ -821,66 +821,66 @@
       <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="11"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="11"/>
+      <c r="C26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C27" s="11"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C28" s="11"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="11"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C30" s="11"/>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C31" s="11"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="11"/>
+      <c r="C32" s="12"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="11"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="11"/>
+      <c r="C34" s="12"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="11"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="11"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="11"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="11"/>
+      <c r="C39" s="12"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="11"/>
+      <c r="C40" s="12"/>
     </row>
     <row r="41" spans="3:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="12"/>
+      <c r="C41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -910,11 +910,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -977,10 +977,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -1053,11 +1053,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1120,10 +1120,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -1196,11 +1196,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1263,10 +1263,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -1339,28 +1339,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1373,17 +1373,17 @@
       <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -1456,10 +1456,10 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -1827,8 +1827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1840,11 +1840,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2009,8 +2009,8 @@
       <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>32</v>
+      <c r="D31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -2061,11 +2061,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2170,9 +2170,9 @@
         <f>'21 Apr'!C31</f>
         <v>Break up project into modules (use UML diagrams)</v>
       </c>
-      <c r="D18" s="1" t="str">
+      <c r="D18" s="1">
         <f>'21 Apr'!D31</f>
-        <v>?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -2279,11 +2279,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2346,10 +2346,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -2464,11 +2464,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2531,10 +2531,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -2607,11 +2607,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2674,10 +2674,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -2750,11 +2750,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2817,10 +2817,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -2893,11 +2893,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2960,10 +2960,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -3036,11 +3036,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -3103,10 +3103,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">

</xml_diff>

<commit_message>
Uploading Scrum Report 4/24.
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hahndol/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepe\IdeaProjects\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E45963B-BE4D-E540-800D-583C486BD173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C5CD04-C7D9-44F4-B95A-E5B3FEB07A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30460" windowHeight="15880" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="44">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Have you ever been bored and wanted something to do to challenge your brain? Well here is the solution for you! Play sudoku today, a free to play game with hours of painful entertainment, and brain exercising. You will have so much fun you will quit all the time! You will enjoy yourself so much while playing this game that you will NEVER recomend it to your friends because you want all of the brain pain to yourself! Enjoy the game! Use the google to figure out what sudoku is so that you can get the best explanation of the game.</t>
+  </si>
+  <si>
+    <t>Aiden</t>
+  </si>
+  <si>
+    <t>Make Print Function for Sudoku</t>
+  </si>
+  <si>
+    <t>Deepesh</t>
+  </si>
+  <si>
+    <t>Write win() method in Sudoku.java</t>
   </si>
 </sst>
 </file>
@@ -175,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +355,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -363,9 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -684,24 +696,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="66.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="66.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -709,7 +721,7 @@
         <v>45036</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -718,7 +730,7 @@
         <v>45037</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -726,7 +738,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -734,7 +746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -742,13 +754,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -756,14 +768,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="123.75" customHeight="1">
       <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -772,7 +784,7 @@
         <v>45037</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -783,7 +795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -794,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -805,7 +817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="s">
         <v>26</v>
       </c>
@@ -816,71 +828,71 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" ht="15" thickBot="1"/>
+    <row r="22" spans="2:4" ht="28.8">
       <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C25" s="11"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="11"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C29" s="11"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C31" s="11"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="11"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" spans="3:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="12"/>
+    <row r="23" spans="2:4">
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="12"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="12"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="12"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="12"/>
+    </row>
+    <row r="41" spans="3:3" ht="15" thickBot="1">
+      <c r="C41" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -901,20 +913,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -922,7 +934,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -943,7 +955,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -952,7 +964,7 @@
         <v>45050</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -960,7 +972,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -968,7 +980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -976,13 +988,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1031,7 @@
         <v>45050</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1044,20 +1056,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1086,7 +1098,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1107,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1123,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1119,13 +1131,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1145,7 +1157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1153,7 +1165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1187,20 +1199,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1208,7 +1220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1229,7 +1241,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1238,7 +1250,7 @@
         <v>45054</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1258,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1266,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1262,13 +1274,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1288,7 +1300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1296,7 +1308,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1317,7 @@
         <v>45054</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1330,39 +1342,39 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1373,19 +1385,19 @@
       <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1422,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1427,7 +1439,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1444,7 +1456,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -1455,11 +1467,11 @@
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -1470,7 +1482,7 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1487,7 +1499,7 @@
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -1498,7 +1510,7 @@
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -1509,7 +1521,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1520,7 +1532,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -1531,7 +1543,7 @@
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -1542,7 +1554,7 @@
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1553,7 +1565,7 @@
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1571,7 +1583,7 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1591,7 +1603,7 @@
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14">
       <c r="C18" t="s">
         <v>25</v>
       </c>
@@ -1608,7 +1620,7 @@
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14">
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
@@ -1619,7 +1631,7 @@
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14">
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
@@ -1630,7 +1642,7 @@
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14">
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -1641,7 +1653,7 @@
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14">
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
@@ -1652,7 +1664,7 @@
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14">
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
@@ -1663,7 +1675,7 @@
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14">
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -1674,7 +1686,7 @@
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14">
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
@@ -1685,7 +1697,7 @@
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14">
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -1696,7 +1708,7 @@
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14">
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
@@ -1707,7 +1719,7 @@
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14">
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
@@ -1718,7 +1730,7 @@
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1736,7 +1748,7 @@
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1753,7 +1765,7 @@
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14">
       <c r="C31" t="s">
         <v>24</v>
       </c>
@@ -1767,7 +1779,7 @@
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14">
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
@@ -1778,7 +1790,7 @@
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:14">
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -1789,7 +1801,7 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:14">
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -1800,7 +1812,7 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:14">
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
@@ -1831,20 +1843,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -1873,7 +1885,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1882,7 +1894,7 @@
         <v>45040</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1890,7 +1902,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1898,7 +1910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1906,13 +1918,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1920,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1932,7 +1944,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1940,7 +1952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" t="str">
         <f>Cover!B18</f>
         <v>All</v>
@@ -1954,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" t="str">
         <f>Cover!B19</f>
         <v>All</v>
@@ -1968,7 +1980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="str">
         <f>Cover!B20</f>
         <v>All</v>
@@ -1982,10 +1994,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="D21" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1994,7 +2006,7 @@
         <v>45040</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
         <v>26</v>
       </c>
@@ -2013,7 +2025,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -2024,7 +2036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -2048,24 +2060,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2073,7 +2085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2094,7 +2106,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2103,7 +2115,7 @@
         <v>45041</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2111,7 +2123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2127,13 +2139,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2141,7 +2153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2153,7 +2165,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" t="str">
         <f>'21 Apr'!B31</f>
         <v>All</v>
@@ -2175,7 +2187,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" t="str">
         <f>'21 Apr'!B32</f>
         <v>TBA</v>
@@ -2189,7 +2201,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" t="str">
         <f>'21 Apr'!B33</f>
         <v>TBA</v>
@@ -2203,7 +2215,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2212,7 +2224,7 @@
         <v>45041</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2220,29 +2232,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -2270,20 +2282,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2291,7 +2303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2312,7 +2324,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2321,7 +2333,7 @@
         <v>45042</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2329,7 +2341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2337,7 +2349,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2345,13 +2357,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2379,35 +2391,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4">
       <c r="B18" t="str">
         <f>'24 Apr'!B31</f>
-        <v>TBA</v>
+        <v>Aiden</v>
       </c>
       <c r="C18" t="str">
         <f>'24 Apr'!C31</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>Make Print Function for Sudoku</v>
+      </c>
+      <c r="D18" s="1">
         <f>'24 Apr'!D31</f>
-        <v>?</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" t="str">
         <f>'24 Apr'!B32</f>
-        <v>TBA</v>
+        <v>Deepesh</v>
       </c>
       <c r="C19" t="str">
         <f>'24 Apr'!C32</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Write win() method in Sudoku.java</v>
+      </c>
+      <c r="D19" s="1">
         <f>'24 Apr'!D32</f>
-        <v>?</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" t="str">
         <f>'24 Apr'!B33</f>
         <v>TBA</v>
@@ -2421,7 +2433,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2430,7 +2442,7 @@
         <v>45042</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2455,20 +2467,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2476,7 +2488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2497,7 +2509,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2506,7 +2518,7 @@
         <v>45043</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2522,7 +2534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2530,13 +2542,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2544,7 +2556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2556,7 +2568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2564,7 +2576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2573,7 +2585,7 @@
         <v>45043</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2598,20 +2610,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2619,7 +2631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2640,7 +2652,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>45044</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2657,7 +2669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2665,7 +2677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2673,13 +2685,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2687,7 +2699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2699,7 +2711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2707,7 +2719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2716,7 +2728,7 @@
         <v>45044</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2741,20 +2753,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2762,7 +2774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2783,7 +2795,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2792,7 +2804,7 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2808,7 +2820,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2816,13 +2828,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2830,7 +2842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2850,7 +2862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2859,7 +2871,7 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2884,20 +2896,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -2905,7 +2917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -2926,7 +2938,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2935,7 +2947,7 @@
         <v>45048</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2951,7 +2963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2959,13 +2971,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2973,7 +2985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2985,7 +2997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2993,7 +3005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3002,7 +3014,7 @@
         <v>45048</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3027,20 +3039,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="23.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="39" customHeight="1">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -3069,7 +3081,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3078,7 +3090,7 @@
         <v>45049</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3086,7 +3098,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3094,7 +3106,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3102,13 +3114,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:14">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3116,7 +3128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3136,7 +3148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3145,7 +3157,7 @@
         <v>45049</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Uploading Scrum Report 4/25.
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepe\IdeaProjects\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD781B2-AE62-4B65-AB56-7ACEFC5DF2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5764AA4C-3F73-4262-863A-9783976EDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="49">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Write reset() method in Sudoku.java</t>
+  </si>
+  <si>
+    <t>Need to add values that are on the board</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -2287,7 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -2392,7 +2398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2400,7 +2406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:5">
       <c r="B18" t="str">
         <f>'24 Apr'!B31</f>
         <v>Aiden</v>
@@ -2413,8 +2419,11 @@
         <f>'24 Apr'!D31</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" t="str">
         <f>'24 Apr'!B32</f>
         <v>Deepesh</v>
@@ -2427,8 +2436,11 @@
         <f>'24 Apr'!D32</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4">
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" t="str">
         <f>'24 Apr'!B33</f>
         <v>TBA</v>
@@ -2442,7 +2454,7 @@
         <v>?</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:5">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2451,7 +2463,7 @@
         <v>45042</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2459,7 +2471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:5">
       <c r="B31" t="s">
         <v>44</v>
       </c>
@@ -2470,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:5">
       <c r="B32" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Uploading Scrum Report 4/27, added colors, print, and set position.
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepe\IdeaProjects\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5764AA4C-3F73-4262-863A-9783976EDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D88FD6-5254-47AE-98F6-4F13C49DEDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="53">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Integrate Print and reset</t>
+  </si>
+  <si>
+    <t>Aiden &amp; Deepesh</t>
+  </si>
+  <si>
+    <t>Work on UI</t>
+  </si>
+  <si>
+    <t>Fix win() method</t>
   </si>
 </sst>
 </file>
@@ -2293,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2504,10 +2516,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2BDEB0-840B-4C3F-B27A-28B18F4DD1A5}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2611,7 +2623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2619,7 +2631,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2628,12 +2668,23 @@
         <v>45043</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2647,10 +2698,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2754,7 +2805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2762,7 +2813,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2771,12 +2836,34 @@
         <v>45044</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading Scrum Report 5/1, finished game
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepe\IdeaProjects\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D88FD6-5254-47AE-98F6-4F13C49DEDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD231E4-9607-4DC6-9263-6E904D74F6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="57">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>Fix win() method</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Deepesh &amp; Aiden</t>
+  </si>
+  <si>
+    <t>Make Presentation for Sudoku</t>
+  </si>
+  <si>
+    <t>Need to add images and text to the slides</t>
   </si>
 </sst>
 </file>
@@ -2700,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2877,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -2984,7 +2996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2992,7 +3004,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3001,12 +3041,23 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3020,10 +3071,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAD585E-1357-492E-B2F5-2576A7D08C49}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -3127,7 +3178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:5">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3135,7 +3186,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3144,12 +3209,23 @@
         <v>45048</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:5">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made it so that the user can restart and create a new board
</commit_message>
<xml_diff>
--- a/ScrumStatusFormswTaskList2023.04.20.xlsx
+++ b/ScrumStatusFormswTaskList2023.04.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepe\IdeaProjects\Sudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DF89C4-1840-43B6-BE64-2618E6D3B82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0021C96-C448-462B-8D4D-20F65A538B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="58">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Need to add images and text to the slides</t>
+  </si>
+  <si>
+    <t>Add a way to quit from the sudoku</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D31486-733F-4C7F-88D0-C517807CD2CE}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1269,6 +1272,17 @@
       </c>
       <c r="D31">
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3148,7 +3162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAD585E-1357-492E-B2F5-2576A7D08C49}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>